<commit_message>
fighting with the recoveries spreadsheet
</commit_message>
<xml_diff>
--- a/Data/DOC/20240201_Readme_NPOC_COMPASS_TEMPEST_EXP_DOC_RECOVERY_Set2.xlsx
+++ b/Data/DOC/20240201_Readme_NPOC_COMPASS_TEMPEST_EXP_DOC_RECOVERY_Set2.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/myer056/GitHub/tempest_ionic_strength/Data/DOC/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5D39AF92-67B6-D444-AC0C-8355813DF425}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AE9FD0A4-A5BC-994C-850A-C2311F8BFA37}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3580" yWindow="760" windowWidth="28420" windowHeight="19920" xr2:uid="{426E503E-EE1F-E344-9DB3-AD0710559367}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="130" uniqueCount="78">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="131" uniqueCount="80">
   <si>
     <t>Sample Name</t>
   </si>
@@ -270,6 +270,12 @@
   </si>
   <si>
     <t xml:space="preserve">GENERAL NOTE: Used the calibration curve from 1/30/2024 STD_0-50ppmNPOC	2, 3, 4, 5, 6, 7, 8, 9, 10		Labeled at 0-10PPM in the instrument curve file name. Slope: 3.457, Int: 0.1588, R2: 1.0000, 0.25ppm and 0.5ppm pt had shouldering but peak areas and rest of curve looked good so retained points		</t>
+  </si>
+  <si>
+    <t>TMP_100.A.2_EXP</t>
+  </si>
+  <si>
+    <t>name was incorrect in the instrument but was 100.A.2 in notebook</t>
   </si>
 </sst>
 </file>
@@ -623,8 +629,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C1E51EA3-AA70-0A4E-9F4C-B0B4A44C6F45}">
   <dimension ref="A1:F72"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="150" workbookViewId="0">
-      <selection activeCell="G71" sqref="G71"/>
+    <sheetView tabSelected="1" topLeftCell="A53" zoomScale="150" workbookViewId="0">
+      <selection activeCell="J65" sqref="J65"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1578,13 +1584,16 @@
     </row>
     <row r="63" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
-        <v>68</v>
+        <v>78</v>
       </c>
       <c r="B63">
         <v>76</v>
       </c>
       <c r="C63" t="s">
         <v>25</v>
+      </c>
+      <c r="D63" t="s">
+        <v>79</v>
       </c>
       <c r="E63">
         <v>230</v>

</xml_diff>